<commit_message>
completed covariate data entry
</commit_message>
<xml_diff>
--- a/data/final_data/de-identified_data.xlsx
+++ b/data/final_data/de-identified_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahgross/Desktop/W241/Final Project/Olive_Oil_Taste_Test/data/final_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8878DA2-FF43-3F42-883E-67340BFEB32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8109B87-A5B9-3143-BCC1-29F89329EB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="18940" windowHeight="14900" xr2:uid="{49F459C7-6492-B94F-B44D-4BE8CD6D4D26}"/>
   </bookViews>
@@ -544,10 +544,10 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2149,6 +2149,9 @@
       <c r="E39" t="s">
         <v>29</v>
       </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
       <c r="G39">
         <v>0</v>
       </c>
@@ -3541,9 +3544,6 @@
         <v>46</v>
       </c>
       <c r="D72" s="1"/>
-      <c r="F72">
-        <v>1</v>
-      </c>
       <c r="J72" t="s">
         <v>13</v>
       </c>

</xml_diff>